<commit_message>
updated to include india
</commit_message>
<xml_diff>
--- a/data/country_representativeness_key.xlsx
+++ b/data/country_representativeness_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrition/subnational_nutrient_distributions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E880AC5D-C4F1-C240-9351-C49A31D86DD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78F1675-51E4-3C44-B603-391B09695360}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30400" yWindow="5420" windowWidth="27640" windowHeight="16940" xr2:uid="{438BE7AA-A47B-1E48-9344-4495C38FC18E}"/>
+    <workbookView xWindow="29680" yWindow="5540" windowWidth="27640" windowHeight="16940" xr2:uid="{438BE7AA-A47B-1E48-9344-4495C38FC18E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>country</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>regional</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>IND</t>
   </si>
 </sst>
 </file>
@@ -582,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05924D41-3461-AD4B-AEA3-2567A8AA0FDD}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,21 +779,21 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>64</v>
@@ -795,10 +801,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>64</v>
@@ -806,76 +812,76 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>63</v>
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" t="s">
-        <v>65</v>
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" t="s">
-        <v>63</v>
+        <v>55</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>64</v>
@@ -883,10 +889,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>64</v>
@@ -894,10 +900,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>64</v>
@@ -905,10 +911,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>64</v>
@@ -916,10 +922,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>64</v>
@@ -927,18 +933,29 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>14</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>15</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C31">
-    <sortCondition ref="A2:A31"/>
+  <sortState ref="A2:C32">
+    <sortCondition ref="A2:A32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>